<commit_message>
added dual specific code
</commit_message>
<xml_diff>
--- a/EEPROM/memory-map.xlsx
+++ b/EEPROM/memory-map.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>Relay 2 behaviour on startup</t>
+  </si>
+  <si>
+    <t>Relay 1 name</t>
+  </si>
+  <si>
+    <t>Relay 2 name</t>
   </si>
 </sst>
 </file>
@@ -478,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,11 +644,11 @@
         <v>2</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" ref="C10:C23" si="4">D9+1</f>
+        <f t="shared" ref="C10:C25" si="4">D9+1</f>
         <v>138</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" ref="D10:D20" si="5">B10+C10-1</f>
+        <f t="shared" ref="D10:D22" si="5">B10+C10-1</f>
         <v>139</v>
       </c>
     </row>
@@ -712,10 +718,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B15" s="2">
-        <v>96</v>
+        <v>16</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="4"/>
@@ -723,156 +729,167 @@
       </c>
       <c r="D15" s="2">
         <f t="shared" si="5"/>
-        <v>239</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B16" s="2">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="4"/>
-        <v>240</v>
+        <v>160</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="5"/>
-        <v>271</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B17" s="2">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="4"/>
-        <v>272</v>
+        <v>176</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="5"/>
-        <v>303</v>
+        <v>239</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" s="2">
         <v>32</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" si="4"/>
-        <v>304</v>
+        <v>240</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="5"/>
-        <v>335</v>
+        <v>271</v>
+      </c>
+      <c r="E18">
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B19" s="2">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C19" s="2">
         <f t="shared" si="4"/>
-        <v>336</v>
+        <v>272</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="5"/>
-        <v>340</v>
+        <v>303</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B20" s="2">
         <v>32</v>
       </c>
       <c r="C20" s="2">
         <f t="shared" si="4"/>
-        <v>341</v>
+        <v>304</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="5"/>
-        <v>372</v>
+        <v>335</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B21" s="2">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="C21" s="2">
         <f t="shared" si="4"/>
-        <v>373</v>
+        <v>336</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" ref="D21:D38" si="6">B21+C21-1</f>
-        <v>404</v>
-      </c>
-      <c r="J21" s="3"/>
+        <f t="shared" si="5"/>
+        <v>340</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B22" s="2">
         <v>32</v>
       </c>
       <c r="C22" s="2">
         <f t="shared" si="4"/>
-        <v>405</v>
+        <v>341</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" si="6"/>
-        <v>436</v>
+        <f t="shared" si="5"/>
+        <v>372</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="2">
+        <v>32</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="4"/>
+        <v>373</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" ref="D23:D40" si="6">B23+C23-1</f>
+        <v>404</v>
+      </c>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="2">
+        <v>32</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="4"/>
+        <v>405</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="6"/>
+        <v>436</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B25" s="2">
         <v>76</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C25" s="2">
         <f t="shared" si="4"/>
         <v>437</v>
-      </c>
-      <c r="D23" s="2">
-        <f t="shared" si="6"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2">
-        <f t="shared" ref="C24:C38" si="7">D23+1</f>
-        <v>513</v>
-      </c>
-      <c r="D24" s="2">
-        <f t="shared" si="6"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2">
-        <f t="shared" si="7"/>
-        <v>513</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="6"/>
@@ -883,7 +900,7 @@
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="C26:C40" si="7">D25+1</f>
         <v>513</v>
       </c>
       <c r="D26" s="2">
@@ -1031,6 +1048,30 @@
         <v>513</v>
       </c>
       <c r="D38" s="2">
+        <f t="shared" si="6"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2">
+        <f t="shared" si="7"/>
+        <v>513</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" si="6"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2">
+        <f t="shared" si="7"/>
+        <v>513</v>
+      </c>
+      <c r="D40" s="2">
         <f t="shared" si="6"/>
         <v>512</v>
       </c>

</xml_diff>

<commit_message>
added second relay methods
</commit_message>
<xml_diff>
--- a/EEPROM/memory-map.xlsx
+++ b/EEPROM/memory-map.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -61,12 +61,6 @@
     <t>MQTT Topic</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Host Name</t>
-  </si>
-  <si>
     <t>DS18B20 present</t>
   </si>
   <si>
@@ -85,9 +79,6 @@
     <t>Relay 2 state</t>
   </si>
   <si>
-    <t>Reserverd</t>
-  </si>
-  <si>
     <t>Relay 1 behaviour on startup</t>
   </si>
   <si>
@@ -98,6 +89,39 @@
   </si>
   <si>
     <t>Relay 2 name</t>
+  </si>
+  <si>
+    <t>Relay 1 behaviour on connection</t>
+  </si>
+  <si>
+    <t>Relay 2 behaviour on connection</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>0.0.0</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>pl,en</t>
+  </si>
+  <si>
+    <t>0-99999</t>
+  </si>
+  <si>
+    <t>1,2,3,4</t>
+  </si>
+  <si>
+    <t>-99.99 - 999.99</t>
+  </si>
+  <si>
+    <t>0-86400</t>
+  </si>
+  <si>
+    <t>Device Name</t>
   </si>
 </sst>
 </file>
@@ -144,7 +168,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -167,18 +191,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -484,18 +526,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,404 +552,444 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
       </c>
       <c r="D2" s="2">
         <f>B2+C2-1</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C9" si="0">D2+1</f>
-        <v>8</v>
+        <f t="shared" ref="C3:C8" si="0">D2+1</f>
+        <v>5</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D4" si="1">B3+C3-1</f>
+        <f t="shared" ref="D3" si="1">B3+C3-1</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="B4" s="2">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <f>B4+C4-1</f>
+        <v>21</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2">
-        <v>96</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2">
-        <f>B5+C5-1</f>
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D5:D6" si="2">B5+C5-1</f>
+        <v>23</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" si="0"/>
-        <v>123</v>
+        <v>24</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" ref="D6:D7" si="2">B6+C6-1</f>
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" si="0"/>
-        <v>124</v>
+        <v>56</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" si="2"/>
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D7:D8" si="3">B7+C7-1</f>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="3"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" ref="C9:C24" si="4">D8+1</f>
+        <v>120</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" ref="D9:D21" si="5">B9+C9-1</f>
+        <v>124</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="4"/>
         <v>125</v>
       </c>
-      <c r="D8" s="2">
-        <f t="shared" ref="D8:D9" si="3">B8+C8-1</f>
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="2">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2">
-        <f t="shared" si="0"/>
-        <v>130</v>
-      </c>
-      <c r="D9" s="2">
-        <f t="shared" si="3"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="2">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2">
-        <f t="shared" ref="C10:C25" si="4">D9+1</f>
-        <v>138</v>
-      </c>
       <c r="D10" s="2">
-        <f t="shared" ref="D10:D22" si="5">B10+C10-1</f>
-        <v>139</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2">
         <f t="shared" si="4"/>
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="5"/>
-        <v>140</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" si="4"/>
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="5"/>
-        <v>141</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C13" s="2">
         <f t="shared" si="4"/>
-        <v>142</v>
+        <v>189</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="5"/>
-        <v>142</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" si="4"/>
-        <v>143</v>
+        <v>205</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="5"/>
-        <v>143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="4"/>
-        <v>144</v>
+        <v>221</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="5"/>
-        <v>159</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B16" s="2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="4"/>
-        <v>160</v>
+        <v>222</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="5"/>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B17" s="2">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="4"/>
-        <v>176</v>
+        <v>223</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="5"/>
-        <v>239</v>
+        <v>223</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" si="4"/>
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="5"/>
-        <v>271</v>
-      </c>
-      <c r="E18">
-        <v>240</v>
+        <v>224</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B19" s="2">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2">
         <f t="shared" si="4"/>
-        <v>272</v>
+        <v>225</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="5"/>
-        <v>303</v>
+        <v>225</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B20" s="2">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2">
         <f t="shared" si="4"/>
-        <v>304</v>
+        <v>226</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="5"/>
-        <v>335</v>
+        <v>226</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B21" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2">
         <f t="shared" si="4"/>
-        <v>336</v>
+        <v>227</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="5"/>
-        <v>340</v>
+        <v>227</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0.1</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B22" s="2">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="C22" s="2">
         <f t="shared" si="4"/>
-        <v>341</v>
+        <v>228</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" si="5"/>
-        <v>372</v>
-      </c>
+        <f t="shared" ref="D22:D39" si="6">B22+C22-1</f>
+        <v>233</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J22" s="3"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B23" s="2">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="C23" s="2">
         <f t="shared" si="4"/>
-        <v>373</v>
+        <v>234</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" ref="D23:D40" si="6">B23+C23-1</f>
-        <v>404</v>
-      </c>
-      <c r="J23" s="3"/>
+        <f t="shared" si="6"/>
+        <v>238</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B24" s="2">
-        <v>32</v>
+        <v>177</v>
       </c>
       <c r="C24" s="2">
         <f t="shared" si="4"/>
-        <v>405</v>
+        <v>239</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="6"/>
-        <v>436</v>
+        <v>415</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25" s="2">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="C25" s="2">
-        <f t="shared" si="4"/>
-        <v>437</v>
+        <f t="shared" ref="C25:C39" si="7">D24+1</f>
+        <v>416</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="6"/>
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2">
-        <f t="shared" ref="C26:C40" si="7">D25+1</f>
-        <v>513</v>
+        <f t="shared" si="7"/>
+        <v>512</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="6"/>
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -913,11 +997,11 @@
       <c r="B27" s="2"/>
       <c r="C27" s="2">
         <f t="shared" si="7"/>
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="6"/>
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -925,11 +1009,11 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2">
         <f t="shared" si="7"/>
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" si="6"/>
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -937,11 +1021,11 @@
       <c r="B29" s="2"/>
       <c r="C29" s="2">
         <f t="shared" si="7"/>
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D29" s="2">
         <f t="shared" si="6"/>
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -949,11 +1033,11 @@
       <c r="B30" s="2"/>
       <c r="C30" s="2">
         <f t="shared" si="7"/>
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" si="6"/>
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -961,11 +1045,11 @@
       <c r="B31" s="2"/>
       <c r="C31" s="2">
         <f t="shared" si="7"/>
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" si="6"/>
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -973,11 +1057,11 @@
       <c r="B32" s="2"/>
       <c r="C32" s="2">
         <f t="shared" si="7"/>
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D32" s="2">
         <f t="shared" si="6"/>
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -985,11 +1069,11 @@
       <c r="B33" s="2"/>
       <c r="C33" s="2">
         <f t="shared" si="7"/>
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D33" s="2">
         <f t="shared" si="6"/>
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -997,11 +1081,11 @@
       <c r="B34" s="2"/>
       <c r="C34" s="2">
         <f t="shared" si="7"/>
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D34" s="2">
         <f t="shared" si="6"/>
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1009,11 +1093,11 @@
       <c r="B35" s="2"/>
       <c r="C35" s="2">
         <f t="shared" si="7"/>
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D35" s="2">
         <f t="shared" si="6"/>
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1021,11 +1105,11 @@
       <c r="B36" s="2"/>
       <c r="C36" s="2">
         <f t="shared" si="7"/>
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D36" s="2">
         <f t="shared" si="6"/>
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1033,11 +1117,11 @@
       <c r="B37" s="2"/>
       <c r="C37" s="2">
         <f t="shared" si="7"/>
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D37" s="2">
         <f t="shared" si="6"/>
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1045,11 +1129,11 @@
       <c r="B38" s="2"/>
       <c r="C38" s="2">
         <f t="shared" si="7"/>
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D38" s="2">
         <f t="shared" si="6"/>
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1057,23 +1141,11 @@
       <c r="B39" s="2"/>
       <c r="C39" s="2">
         <f t="shared" si="7"/>
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D39" s="2">
         <f t="shared" si="6"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2">
-        <f t="shared" si="7"/>
-        <v>513</v>
-      </c>
-      <c r="D40" s="2">
-        <f t="shared" si="6"/>
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
   </sheetData>

</xml_diff>